<commit_message>
resolving #45 resolving #42 continuing object properties, and getters setters etc
</commit_message>
<xml_diff>
--- a/followMe/mDB files/fm_objects.xlsx
+++ b/followMe/mDB files/fm_objects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvsib\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvsib\Source\Repos\followMe\followMe\mDB files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -577,8 +577,8 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G31:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
       </c>
       <c r="I1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1">
         <f t="shared" si="0"/>
@@ -1246,7 +1246,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1267,14 +1267,14 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
         <f>COUNTIF(C19:J19,1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <f>COUNTIF(C22:J22,1)</f>
+        <f t="shared" ref="K22:K38" si="2">COUNTIF(C22:J22,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <f>COUNTIF(C23:J23,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <f>COUNTIF(C24:J24,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <f>COUNTIF(C25:J25,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <f>COUNTIF(C26:J26,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <f>COUNTIF(C27:J27,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <f>COUNTIF(C28:J28,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f>COUNTIF(C29:J29,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L29" t="s">
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <f>COUNTIF(C30:J30,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L30" t="s">
@@ -1711,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <f>COUNTIF(C31:J31,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <f>COUNTIF(C32:J32,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1783,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <f>COUNTIF(C33:J33,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <f>COUNTIF(C34:J34,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <f>COUNTIF(C35:J35,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L35" t="s">
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <f>COUNTIF(C36:J36,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L36" t="s">
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <f>COUNTIF(C37:J37,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L37" t="s">
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <f>COUNTIF(C38:J38,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L38" t="s">

</xml_diff>

<commit_message>
resolving #48 resolving #45 resolving #42 concept of typeScript classes, and server based addition has started, will require much more cleaning up and further object declaration. E.g. _id needs to be the unique ID
</commit_message>
<xml_diff>
--- a/followMe/mDB files/fm_objects.xlsx
+++ b/followMe/mDB files/fm_objects.xlsx
@@ -577,20 +577,20 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G31:G33"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="12" width="4.140625" customWidth="1"/>
@@ -599,34 +599,34 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C1">
         <f>COUNTIF(C3:C38,1)</f>
+        <v>15</v>
+      </c>
+      <c r="D1">
+        <f>COUNTIF(D3:D38,1)</f>
         <v>3</v>
       </c>
-      <c r="D1">
-        <f t="shared" ref="D1:J1" si="0">COUNTIF(D3:D38,1)</f>
+      <c r="E1">
+        <f>COUNTIF(E3:E38,1)</f>
         <v>21</v>
       </c>
-      <c r="E1">
-        <f t="shared" si="0"/>
+      <c r="F1">
+        <f>COUNTIF(F3:F38,1)</f>
         <v>3</v>
       </c>
-      <c r="F1">
-        <f t="shared" si="0"/>
+      <c r="G1">
+        <f>COUNTIF(G3:G38,1)</f>
         <v>13</v>
       </c>
-      <c r="G1">
-        <f t="shared" si="0"/>
+      <c r="H1">
+        <f>COUNTIF(H3:H38,1)</f>
         <v>13</v>
       </c>
-      <c r="H1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
       <c r="I1">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(I3:I38,1)</f>
         <v>19</v>
       </c>
       <c r="J1">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(J3:J38,1)</f>
         <v>19</v>
       </c>
     </row>
@@ -635,22 +635,22 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>38</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
       </c>
       <c r="I2" t="s">
         <v>40</v>
@@ -697,8 +697,8 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K21" si="1">COUNTIF(C3:J3,1)</f>
-        <v>8</v>
+        <f>COUNTIF(D3:J3,1)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -733,8 +733,8 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f>COUNTIF(D4:J4,1)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -745,16 +745,16 @@
         <v>49</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -769,8 +769,8 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D5:J5,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -781,16 +781,16 @@
         <v>49</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -805,8 +805,8 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D6:J6,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -817,16 +817,16 @@
         <v>49</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -841,8 +841,8 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D7:J7,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -853,16 +853,16 @@
         <v>49</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -877,8 +877,8 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D8:J8,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -889,16 +889,16 @@
         <v>49</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -913,8 +913,8 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D9:J9,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -925,16 +925,16 @@
         <v>49</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -949,8 +949,8 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D10:J10,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -961,16 +961,16 @@
         <v>49</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -985,8 +985,8 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D11:J11,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -997,16 +997,16 @@
         <v>49</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1021,8 +1021,8 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>COUNTIF(D12:J12,1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1033,13 +1033,13 @@
         <v>51</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1048,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1057,8 +1057,8 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>COUNTIF(D13:J13,1)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1069,13 +1069,13 @@
         <v>51</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1093,8 +1093,8 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>COUNTIF(D14:J14,1)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1105,13 +1105,13 @@
         <v>51</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1129,8 +1129,8 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>COUNTIF(D15:J15,1)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1141,13 +1141,13 @@
         <v>51</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1165,8 +1165,8 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>COUNTIF(D16:J16,1)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1180,10 +1180,10 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1201,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(D17:J17,1)</f>
         <v>3</v>
       </c>
     </row>
@@ -1216,10 +1216,10 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(D18:J18,1)</f>
         <v>3</v>
       </c>
     </row>
@@ -1246,16 +1246,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1273,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <f>COUNTIF(C19:J19,1)</f>
+        <f>COUNTIF(D19:J19,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1285,19 +1285,19 @@
         <v>63</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1309,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(D20:J20,1)</f>
         <v>3</v>
       </c>
     </row>
@@ -1324,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1333,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(D21:J21,1)</f>
         <v>3</v>
       </c>
     </row>
@@ -1360,10 +1360,10 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:K38" si="2">COUNTIF(C22:J22,1)</f>
+        <f t="shared" ref="K22:K38" si="0">COUNTIF(D22:J22,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1429,7 +1429,7 @@
         <v>61</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1453,8 +1453,8 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1540,10 +1540,10 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1582,10 +1582,10 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1597,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L29" t="s">
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L30" t="s">
@@ -1699,10 +1699,10 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -1711,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1735,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1771,10 +1771,10 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L35" t="s">
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L36" t="s">
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L37" t="s">
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L38" t="s">

</xml_diff>

<commit_message>
continuing classess in typescript
</commit_message>
<xml_diff>
--- a/followMe/mDB files/fm_objects.xlsx
+++ b/followMe/mDB files/fm_objects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvsib\Source\Repos\followMe\followMe\mDB files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent.Norris\Source\Repos\followMe\followMe\mDB files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
   <si>
     <t>ObjectId _id</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Player?</t>
   </si>
   <si>
-    <t>remove, declared by level</t>
-  </si>
-  <si>
     <t>removed, unique ID is above</t>
   </si>
   <si>
@@ -223,13 +220,70 @@
   </si>
   <si>
     <t>animatedMovementGameObject</t>
+  </si>
+  <si>
+    <t>Objects req'd</t>
+  </si>
+  <si>
+    <t>Objects set</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>Checkpoint</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Cave</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>lives</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Needs review for properties</t>
+  </si>
+  <si>
+    <t>Has all properties</t>
+  </si>
+  <si>
+    <t>Not added</t>
+  </si>
+  <si>
+    <t>local</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,16 +291,73 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -254,14 +365,138 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,104 +809,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89087116-E83A-42DE-B1EF-B8C1A7B0DD24}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="12" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C1">
-        <f>COUNTIF(C3:C38,1)</f>
+        <f>COUNTIF(C3:C43,1)</f>
         <v>15</v>
       </c>
       <c r="D1">
-        <f>COUNTIF(D3:D38,1)</f>
+        <f>COUNTIF(D3:D43,1)</f>
+        <v>21</v>
+      </c>
+      <c r="E1">
+        <f>COUNTIF(E3:E43,1)</f>
+        <v>17</v>
+      </c>
+      <c r="F1">
+        <f>COUNTIF(F3:F43,1)</f>
+        <v>13</v>
+      </c>
+      <c r="G1">
+        <f>COUNTIF(G3:G43,1)</f>
         <v>3</v>
       </c>
-      <c r="E1">
-        <f>COUNTIF(E3:E38,1)</f>
-        <v>21</v>
-      </c>
-      <c r="F1">
-        <f>COUNTIF(F3:F38,1)</f>
-        <v>3</v>
-      </c>
-      <c r="G1">
-        <f>COUNTIF(G3:G38,1)</f>
+      <c r="H1">
+        <f>COUNTIF(H3:H43,1)</f>
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <f>COUNTIF(I3:I43,1)</f>
         <v>13</v>
       </c>
-      <c r="H1">
-        <f>COUNTIF(H3:H38,1)</f>
-        <v>13</v>
-      </c>
-      <c r="I1">
-        <f>COUNTIF(I3:I38,1)</f>
-        <v>19</v>
-      </c>
       <c r="J1">
-        <f>COUNTIF(J3:J38,1)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(J3:J43,1)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
       <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>46</v>
       </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
       <c r="C3">
         <v>1</v>
       </c>
@@ -697,16 +936,16 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <f>COUNTIF(D3:J3,1)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(G3:J3,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>48</v>
+      <c r="B4" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -733,34 +972,34 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f>COUNTIF(D4:J4,1)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(G4:J4,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>49</v>
+      <c r="B5" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -769,34 +1008,34 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f>COUNTIF(D5:J5,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(G5:J5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>49</v>
+      <c r="B6" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -805,34 +1044,34 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <f>COUNTIF(D6:J6,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(G6:J6,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
+      <c r="B7" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -841,34 +1080,34 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <f>COUNTIF(D7:J7,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(G7:J7,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
-        <v>49</v>
+      <c r="B8" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -877,34 +1116,34 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <f>COUNTIF(D8:J8,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(G8:J8,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
+      <c r="B9" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -913,34 +1152,34 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f>COUNTIF(D9:J9,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(G9:J9,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
-        <v>49</v>
+      <c r="B10" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -949,34 +1188,34 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f>COUNTIF(D10:J10,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C10:J10,1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
-        <v>49</v>
+      <c r="B11" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -985,34 +1224,34 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f>COUNTIF(D11:J11,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C11:J11,1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
-        <v>49</v>
+      <c r="B12" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1021,22 +1260,22 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <f>COUNTIF(D12:J12,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C12:J12,1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>51</v>
+      <c r="B13" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1051,28 +1290,28 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13">
-        <f>COUNTIF(D13:J13,1)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C13:J13,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>51</v>
+      <c r="B14" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1087,28 +1326,28 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <f>COUNTIF(D14:J14,1)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C14:J14,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
-        <v>51</v>
+      <c r="B15" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1123,28 +1362,28 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15">
-        <f>COUNTIF(D15:J15,1)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C15:J15,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
-        <v>51</v>
+      <c r="B16" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1159,31 +1398,31 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16">
-        <f>COUNTIF(D16:J16,1)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C16:J16,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>64</v>
+      <c r="B17" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1195,31 +1434,31 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <f>COUNTIF(D17:J17,1)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C17:J17,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
-        <v>64</v>
+      <c r="B18" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1231,31 +1470,31 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <f>COUNTIF(D18:J18,1)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C18:J18,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>64</v>
+      <c r="B19" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1273,16 +1512,16 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <f>COUNTIF(D19:J19,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C19:J19,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>63</v>
+      <c r="B20" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1291,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1309,34 +1548,40 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <f>COUNTIF(D20:J20,1)</f>
+        <f>COUNTIF(C20:J20,1)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
-        <v>62</v>
+      <c r="B21" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1345,25 +1590,35 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <f>COUNTIF(D21:J21,1)</f>
+        <f>COUNTIF(C21:J21,1)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="7" t="str">
+        <f>IF(ISNA(VLOOKUP(M21,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" t="s">
-        <v>60</v>
+      <c r="B22" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1381,16 +1636,26 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:K38" si="0">COUNTIF(D22:J22,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C22:J22,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M22,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
+      <c r="B23" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1399,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1411,22 +1676,32 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C23:J23,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N23" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M23,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="B24" t="s">
-        <v>61</v>
+      <c r="B24" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1453,15 +1728,22 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C24:J24,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N24" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M24,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C25">
@@ -1471,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1483,21 +1765,28 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C25:J25,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N25" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M25,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C26">
@@ -1507,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1519,31 +1808,38 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C26:J26,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N26" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M26,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B27" t="s">
-        <v>60</v>
+      <c r="B27" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1561,16 +1857,23 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C27:J27,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N27" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M27,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" t="s">
-        <v>59</v>
+      <c r="B28" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1582,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1597,16 +1900,23 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C28:J28,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="N28" s="12" t="str">
+        <f>IF(ISNA(VLOOKUP(M28,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1633,19 +1943,16 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C29:J29,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1672,19 +1979,16 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C30:J30,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1702,25 +2006,25 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31">
         <v>0</v>
       </c>
       <c r="K31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C31:J31,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1738,16 +2042,16 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(C32:J32,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1756,7 +2060,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1774,25 +2078,25 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33">
         <v>0</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C33:J33,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1819,13 +2123,16 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <f>COUNTIF(C34:J34,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>74</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1843,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -1852,16 +2159,16 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="K35:K39" si="0">COUNTIF(C35:J35,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1879,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -1889,15 +2196,15 @@
       </c>
       <c r="K36">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>75</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1915,7 +2222,7 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -1925,15 +2232,15 @@
       </c>
       <c r="K37">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>76</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1951,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -1961,19 +2268,208 @@
       </c>
       <c r="K38">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L38" t="s">
-        <v>56</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f>COUNTIF(C40:J40,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <f>COUNTIF(C41:J41,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f>COUNTIF(C42:J42,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f>COUNTIF(C43:J43,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L43" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:L2" xr:uid="{93EF88EE-FD76-4978-8475-178602C9994F}">
-    <sortState ref="A3:L38">
+    <sortState ref="A3:L43">
       <sortCondition descending="1" ref="K2"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C3:J38">
+  <conditionalFormatting sqref="C3:J43">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1984,6 +2480,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2006,37 +2503,37 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2046,7 +2543,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2056,17 +2553,17 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolving #45 resolving #42 full class implementation, and removal of index or uniqueidentifier, just using _id instead. Will move to changing logic to use new classes
</commit_message>
<xml_diff>
--- a/followMe/mDB files/fm_objects.xlsx
+++ b/followMe/mDB files/fm_objects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent.Norris\Source\Repos\followMe\followMe\mDB files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvsib\Source\Repos\followMe\followMe\mDB files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>ObjectId _id</t>
   </si>
@@ -192,12 +192,6 @@
     <t>animatedHurtingGameObject</t>
   </si>
   <si>
-    <t>should be xend</t>
-  </si>
-  <si>
-    <t>should be yend</t>
-  </si>
-  <si>
     <t>cave</t>
   </si>
   <si>
@@ -277,6 +271,12 @@
   </si>
   <si>
     <t>local</t>
+  </si>
+  <si>
+    <t>teleportAllowed</t>
+  </si>
+  <si>
+    <t>Image specific movement</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -487,10 +487,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -809,11 +808,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89087116-E83A-42DE-B1EF-B8C1A7B0DD24}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,36 +836,36 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C1">
-        <f>COUNTIF(C3:C43,1)</f>
+        <f>COUNTIF(C3:C44,1)</f>
         <v>15</v>
       </c>
       <c r="D1">
-        <f>COUNTIF(D3:D43,1)</f>
-        <v>21</v>
+        <f>COUNTIF(D3:D44,1)</f>
+        <v>22</v>
       </c>
       <c r="E1">
-        <f>COUNTIF(E3:E43,1)</f>
+        <f>COUNTIF(E3:E44,1)</f>
         <v>17</v>
       </c>
       <c r="F1">
-        <f>COUNTIF(F3:F43,1)</f>
-        <v>13</v>
+        <f>COUNTIF(F3:F44,1)</f>
+        <v>14</v>
       </c>
       <c r="G1">
-        <f>COUNTIF(G3:G43,1)</f>
+        <f>COUNTIF(G3:G44,1)</f>
         <v>3</v>
       </c>
       <c r="H1">
-        <f>COUNTIF(H3:H43,1)</f>
-        <v>8</v>
+        <f>COUNTIF(H3:H44,1)</f>
+        <v>10</v>
       </c>
       <c r="I1">
-        <f>COUNTIF(I3:I43,1)</f>
-        <v>13</v>
+        <f>COUNTIF(I3:I44,1)</f>
+        <v>14</v>
       </c>
       <c r="J1">
-        <f>COUNTIF(J3:J43,1)</f>
-        <v>17</v>
+        <f>COUNTIF(J3:J44,1)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -908,7 +907,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C3">
@@ -936,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <f>COUNTIF(G3:J3,1)</f>
+        <f t="shared" ref="K3:K9" si="0">COUNTIF(G3:J3,1)</f>
         <v>4</v>
       </c>
     </row>
@@ -944,7 +943,7 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C4">
@@ -972,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f>COUNTIF(G4:J4,1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -980,7 +979,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C5">
@@ -1008,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f>COUNTIF(G5:J5,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1016,7 +1015,7 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C6">
@@ -1044,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <f>COUNTIF(G6:J6,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1052,7 +1051,7 @@
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C7">
@@ -1080,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <f>COUNTIF(G7:J7,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1088,7 +1087,7 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C8">
@@ -1116,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <f>COUNTIF(G8:J8,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1124,7 +1123,7 @@
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C9">
@@ -1152,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f>COUNTIF(G9:J9,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1160,7 +1159,7 @@
       <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C10">
@@ -1188,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f>COUNTIF(C10:J10,1)</f>
+        <f t="shared" ref="K10:K35" si="1">COUNTIF(C10:J10,1)</f>
         <v>6</v>
       </c>
     </row>
@@ -1196,7 +1195,7 @@
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C11">
@@ -1224,7 +1223,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f>COUNTIF(C11:J11,1)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1232,7 +1231,7 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C12">
@@ -1260,16 +1259,16 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <f>COUNTIF(C12:J12,1)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1281,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1290,21 +1289,21 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13">
         <f>COUNTIF(C13:J13,1)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C14">
@@ -1332,15 +1331,15 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <f>COUNTIF(C14:J14,1)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C15">
@@ -1368,15 +1367,15 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <f>COUNTIF(C15:J15,1)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C16">
@@ -1404,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <f>COUNTIF(C16:J16,1)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1412,8 +1411,8 @@
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>63</v>
+      <c r="B17" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1440,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <f>COUNTIF(C17:J17,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1448,8 +1447,8 @@
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>63</v>
+      <c r="B18" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1476,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <f>COUNTIF(C18:J18,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1484,8 +1483,8 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>63</v>
+      <c r="B19" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1512,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <f>COUNTIF(C19:J19,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1520,50 +1519,50 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <f>COUNTIF(C20:J20,1)</f>
-        <v>3</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="N20" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>61</v>
+      <c r="B21" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1590,26 +1589,26 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <f>COUNTIF(C21:J21,1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N21" s="7" t="str">
-        <f>IF(ISNA(VLOOKUP(M21,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M21,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>59</v>
+      <c r="B22" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1636,25 +1635,25 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <f>COUNTIF(C22:J22,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N22" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M22,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M22,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C23">
@@ -1682,26 +1681,26 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <f>COUNTIF(C23:J23,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N23" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M23,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M23,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>60</v>
+      <c r="B24" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1728,14 +1727,14 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <f>COUNTIF(C24:J24,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N24" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M24,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M24,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
@@ -1743,7 +1742,7 @@
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C25">
@@ -1771,14 +1770,14 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <f>COUNTIF(C25:J25,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N25" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M25,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M25,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
@@ -1786,7 +1785,7 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C26">
@@ -1814,14 +1813,14 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <f>COUNTIF(C26:J26,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N26" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M26,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M26,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
@@ -1829,8 +1828,8 @@
       <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>59</v>
+      <c r="B27" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1857,14 +1856,14 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <f>COUNTIF(C27:J27,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M27" s="10" t="s">
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="N27" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M27,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M27,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
@@ -1872,8 +1871,8 @@
       <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>58</v>
+      <c r="B28" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1900,23 +1899,23 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <f>COUNTIF(C28:J28,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M28" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="N28" s="12" t="str">
-        <f>IF(ISNA(VLOOKUP(M28,$B$3:$B$43,1,FALSE)),"no","yes")</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N28" s="10" t="str">
+        <f>IF(ISNA(VLOOKUP(M28,$B$3:$B$44,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" t="s">
-        <v>57</v>
+      <c r="B29" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1943,16 +1942,16 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f>COUNTIF(C29:J29,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B30" t="s">
-        <v>57</v>
+      <c r="B30" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1979,16 +1978,16 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <f>COUNTIF(C30:J30,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2009,94 +2008,90 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <f>COUNTIF(C31:J31,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <f>COUNTIF(C32:J32,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <f>COUNTIF(C33:J33,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>57</v>
+      <c r="B34" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2117,22 +2112,22 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34">
-        <f>COUNTIF(C34:J34,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>77</v>
+        <v>32</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2150,25 +2145,25 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35">
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K39" si="0">COUNTIF(C35:J35,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>77</v>
+        <v>27</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2195,16 +2190,19 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>COUNTIF(C36:J36,1)</f>
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>77</v>
+        <v>28</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2231,16 +2229,19 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>COUNTIF(C37:J37,1)</f>
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2267,16 +2268,16 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K38:K42" si="2">COUNTIF(C38:J38,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>77</v>
+        <v>21</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2303,133 +2304,124 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>2</v>
       </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <f>COUNTIF(C40:J40,1)</f>
-        <v>0</v>
-      </c>
-      <c r="L40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <f>COUNTIF(C41:J41,1)</f>
-        <v>0</v>
-      </c>
-      <c r="L41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <f>COUNTIF(C42:J42,1)</f>
-        <v>0</v>
-      </c>
-      <c r="L42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>28</v>
-      </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2460,17 +2452,76 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>55</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f>COUNTIF(C44:J44,1)</f>
+        <v>1</v>
+      </c>
+      <c r="L44" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:L2" xr:uid="{93EF88EE-FD76-4978-8475-178602C9994F}">
-    <sortState ref="A3:L43">
+    <sortState ref="A3:L44">
       <sortCondition descending="1" ref="K2"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C3:J43">
+  <conditionalFormatting sqref="C31:J31">
     <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:J32">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:J30 C33:J44">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2528,12 +2579,12 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2543,7 +2594,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2553,17 +2604,17 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolving #45 resolving #42 closing #52 followMe.surfaces uses typescript classes, buildLevel will need more cleanup, and UI will need to be included in typescript code instead, which is next
</commit_message>
<xml_diff>
--- a/followMe/mDB files/fm_objects.xlsx
+++ b/followMe/mDB files/fm_objects.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>ObjectId _id</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>Image specific movement</t>
+  </si>
+  <si>
+    <t>maxx</t>
+  </si>
+  <si>
+    <t>maxy</t>
+  </si>
+  <si>
+    <t>used for collision</t>
   </si>
 </sst>
 </file>
@@ -329,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +363,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -476,7 +491,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -490,6 +505,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -808,11 +824,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89087116-E83A-42DE-B1EF-B8C1A7B0DD24}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36:B37"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,35 +852,35 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C1">
-        <f>COUNTIF(C3:C44,1)</f>
+        <f>COUNTIF(C3:C46,1)</f>
         <v>15</v>
       </c>
       <c r="D1">
-        <f>COUNTIF(D3:D44,1)</f>
-        <v>22</v>
+        <f>COUNTIF(D3:D46,1)</f>
+        <v>23</v>
       </c>
       <c r="E1">
-        <f>COUNTIF(E3:E44,1)</f>
+        <f>COUNTIF(E3:E46,1)</f>
         <v>17</v>
       </c>
       <c r="F1">
-        <f>COUNTIF(F3:F44,1)</f>
+        <f>COUNTIF(F3:F46,1)</f>
         <v>14</v>
       </c>
       <c r="G1">
-        <f>COUNTIF(G3:G44,1)</f>
+        <f>COUNTIF(G3:G46,1)</f>
         <v>3</v>
       </c>
       <c r="H1">
-        <f>COUNTIF(H3:H44,1)</f>
+        <f>COUNTIF(H3:H46,1)</f>
         <v>10</v>
       </c>
       <c r="I1">
-        <f>COUNTIF(I3:I44,1)</f>
+        <f>COUNTIF(I3:I46,1)</f>
         <v>14</v>
       </c>
       <c r="J1">
-        <f>COUNTIF(J3:J44,1)</f>
+        <f>COUNTIF(J3:J46,1)</f>
         <v>18</v>
       </c>
     </row>
@@ -1187,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K35" si="1">COUNTIF(C10:J10,1)</f>
+        <f t="shared" ref="K10:K37" si="1">COUNTIF(C10:J10,1)</f>
         <v>6</v>
       </c>
     </row>
@@ -1596,7 +1612,7 @@
         <v>64</v>
       </c>
       <c r="N21" s="7" t="str">
-        <f>IF(ISNA(VLOOKUP(M21,$B$3:$B$44,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M21,$B$3:$B$46,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
       <c r="P21" s="3" t="s">
@@ -1642,7 +1658,7 @@
         <v>65</v>
       </c>
       <c r="N22" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M22,$B$3:$B$44,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M22,$B$3:$B$46,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
       <c r="P22" s="2" t="s">
@@ -1651,108 +1667,94 @@
     </row>
     <row r="23" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
+        <v>57</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
+        <v>0</v>
+      </c>
+      <c r="J23" s="13">
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="N23" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M23,$B$3:$B$44,1,FALSE)),"no","yes")</f>
-        <v>yes</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>78</v>
+        <f t="shared" ref="K23:K24" si="2">COUNTIF(C23:J23,1)</f>
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
+        <v>57</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0</v>
+      </c>
+      <c r="D24" s="13">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <v>0</v>
+      </c>
+      <c r="I24" s="13">
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M24,$B$3:$B$44,1,FALSE)),"no","yes")</f>
-        <v>yes</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1770,32 +1772,32 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(C25:J25,1)</f>
         <v>1</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N25" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M25,$B$3:$B$44,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M25,$B$3:$B$46,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1813,32 +1815,32 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(C26:J26,1)</f>
         <v>1</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N26" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M26,$B$3:$B$44,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M26,$B$3:$B$46,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1860,19 +1862,22 @@
         <v>1</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N27" s="9" t="str">
-        <f>IF(ISNA(VLOOKUP(M27,$B$3:$B$44,1,FALSE)),"no","yes")</f>
+        <f>IF(ISNA(VLOOKUP(M27,$B$3:$B$46,1,FALSE)),"no","yes")</f>
         <v>yes</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1881,10 +1886,10 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1902,20 +1907,20 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M28" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="N28" s="10" t="str">
-        <f>IF(ISNA(VLOOKUP(M28,$B$3:$B$44,1,FALSE)),"no","yes")</f>
+      <c r="M28" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N28" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M28,$B$3:$B$46,1,FALSE)),"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1924,7 +1929,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1939,19 +1944,26 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="M29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N29" s="9" t="str">
+        <f>IF(ISNA(VLOOKUP(M29,$B$3:$B$46,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
     </row>
     <row r="30" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1963,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1975,16 +1987,23 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="M30" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N30" s="10" t="str">
+        <f>IF(ISNA(VLOOKUP(M30,$B$3:$B$46,1,FALSE)),"no","yes")</f>
+        <v>yes</v>
+      </c>
     </row>
     <row r="31" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>55</v>
@@ -2014,13 +2033,13 @@
         <v>1</v>
       </c>
       <c r="K31">
-        <f>COUNTIF(C31:J31,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>55</v>
@@ -2049,13 +2068,17 @@
       <c r="J32">
         <v>1</v>
       </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2076,22 +2099,22 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(C33:J33,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2112,19 +2135,15 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>54</v>
@@ -2160,7 +2179,7 @@
     </row>
     <row r="36" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>54</v>
@@ -2181,25 +2200,22 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
       <c r="K36">
-        <f>COUNTIF(C36:J36,1)</f>
-        <v>1</v>
-      </c>
-      <c r="L36" t="s">
-        <v>82</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>54</v>
@@ -2220,28 +2236,25 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37">
         <v>0</v>
       </c>
       <c r="K37">
-        <f>COUNTIF(C37:J37,1)</f>
-        <v>1</v>
-      </c>
-      <c r="L37" t="s">
-        <v>82</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2268,16 +2281,19 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" ref="K38:K42" si="2">COUNTIF(C38:J38,1)</f>
-        <v>1</v>
+        <f>COUNTIF(C38:J38,1)</f>
+        <v>1</v>
+      </c>
+      <c r="L38" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2304,13 +2320,16 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>COUNTIF(C39:J39,1)</f>
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>75</v>
@@ -2340,13 +2359,13 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K40:K44" si="3">COUNTIF(C40:J40,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>75</v>
@@ -2376,13 +2395,13 @@
         <v>0</v>
       </c>
       <c r="K41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>75</v>
@@ -2412,116 +2431,168 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B45" t="s">
         <v>76</v>
       </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <f>COUNTIF(C43:J43,1)</f>
-        <v>0</v>
-      </c>
-      <c r="L43" t="s">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <f>COUNTIF(C45:J45,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>22</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>76</v>
       </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <f>COUNTIF(C44:J44,1)</f>
-        <v>1</v>
-      </c>
-      <c r="L44" t="s">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <f>COUNTIF(C46:J46,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L46" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:L2" xr:uid="{93EF88EE-FD76-4978-8475-178602C9994F}">
-    <sortState ref="A3:L44">
+    <sortState ref="A3:L46">
       <sortCondition descending="1" ref="K2"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C31:J31">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:J32">
+  <conditionalFormatting sqref="C3:J46">
     <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:J30 C33:J44">
-    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>